<commit_message>
Updated sheet 'Sheet1' with new data
</commit_message>
<xml_diff>
--- a/empty.xlsx
+++ b/empty.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,62 +436,242 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Item</t>
+          <t>MIGRATION DATE</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Client Setting/Value</t>
+          <t>FINANCIAL INSTITUTION NAME</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ENTITY ID</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ADDRESS</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>CITY</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>STATE</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ZIP CODE</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>PHONE #</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>PROJECT COORDINATOR</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>CERTIFICATION REQUIRED (Yes or No)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>CERTIFICATION COORDINATOR</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Migration Date</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
           <t>2025-10-16</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Entity ID</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
+          <t>YYY</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>123ABX007</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Financial Institution</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>YYY</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>City</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Karapakkam</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
         <is>
           <t>Chennai</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Tamil Nadu</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>600117</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>9911991100</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Sam</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated sheet 'Sheet1' with key-value data (no headers)
</commit_message>
<xml_diff>
--- a/empty.xlsx
+++ b/empty.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,244 +422,132 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>MIGRATION DATE</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>FINANCIAL INSTITUTION NAME</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>ENTITY ID</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>ADDRESS</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>CITY</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>STATE</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>ZIP CODE</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>PHONE #</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>PROJECT COORDINATOR</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>CERTIFICATION REQUIRED (Yes or No)</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>CERTIFICATION COORDINATOR</t>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>2025-10-16</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+          <t>FINANCIAL INSTITUTION NAME</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>YYY</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ENTITY ID</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>YYY</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+          <t>123ABX007</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>123ABX007</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ADDRESS</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Karapakkam</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Karapakkam</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CITY</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Chennai</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>STATE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Tamil Nadu</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Tamil Nadu</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ZIP CODE</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>600117</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>600117</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PHONE #</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>9911991100</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>9911991100</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>PROJECT COORDINATOR</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Sam</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>Sam</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>CERTIFICATION REQUIRED (Yes or No)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>CERTIFICATION COORDINATOR</t>
+        </is>
+      </c>
       <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Appended data to sheet 'Sheet1'
</commit_message>
<xml_diff>
--- a/empty.xlsx
+++ b/empty.xlsx
@@ -1,53 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivek.lade\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2182990-C49B-458D-B646-EB61D3CF2779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -55,44 +42,85 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -380,18 +408,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>MIGRATION DATE</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>FINANCIAL INSTITUTION NAME</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ENTITY ID</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>ADDRESS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-10-16</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>YYY</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>123ABX007</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Karapakkam</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Appended new data to 'Sheet1'
</commit_message>
<xml_diff>
--- a/empty.xlsx
+++ b/empty.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,6 +499,28 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-10-17</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ZZZ</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>456CDX009</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Anna Nagar</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Appended data to 'Sheet1'
</commit_message>
<xml_diff>
--- a/empty.xlsx
+++ b/empty.xlsx
@@ -1,47 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivek.lade\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2182990-C49B-458D-B646-EB61D3CF2779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -56,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -380,18 +420,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>MIGRATION DATE</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>FINANCIAL INSTITUTION NAME</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ENTITY ID</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ADDRESS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-10-17</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ZZZ</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>456CDX009</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Anna Nagar</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Appended/Updated data to 'Sheet1'
</commit_message>
<xml_diff>
--- a/empty.xlsx
+++ b/empty.xlsx
@@ -481,11 +481,7 @@
           <t>AAA</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Chennai</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">

</xml_diff>